<commit_message>
Fixed processing hardcoded function
</commit_message>
<xml_diff>
--- a/main/app/brm_core/BRMRulesLatest.xlsx
+++ b/main/app/brm_core/BRMRulesLatest.xlsx
@@ -110,12 +110,6 @@
     <t>STATION &lt; 9999</t>
   </si>
   <si>
-    <t xml:space="preserve">CAR_SERIES &lt;=  'MILW120209' </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAR_SERIES  &gt;=  'MILW120000' </t>
-  </si>
-  <si>
     <t xml:space="preserve"> starts_with(AAR_CAR_TYPE, "T")</t>
   </si>
   <si>
@@ -126,6 +120,12 @@
   </si>
   <si>
     <t>AAR_CAR_TYPE,CAR_SERIES,SCS</t>
+  </si>
+  <si>
+    <t>exclude(CAR_SERIES ,"MILW") &lt;= 120209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exclude(CAR_SERIES ,"MILW" )&gt;= 120000 </t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +534,8 @@
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="5" width="43.42578125" customWidth="1"/>
+    <col min="4" max="4" width="52.140625" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" customWidth="1"/>
     <col min="6" max="7" width="23.85546875" customWidth="1"/>
     <col min="8" max="8" width="47.7109375" customWidth="1"/>
   </cols>
@@ -547,10 +548,10 @@
         <v>17</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>6</v>
@@ -603,10 +604,10 @@
         <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -656,10 +657,10 @@
         <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>5</v>
@@ -709,10 +710,10 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -856,7 +857,7 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Fixed start_with embedded function to be more flexible on arguments
</commit_message>
<xml_diff>
--- a/main/app/brm_core/BRMRulesLatest.xlsx
+++ b/main/app/brm_core/BRMRulesLatest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="48">
   <si>
     <t>None</t>
   </si>
@@ -78,54 +78,135 @@
     <t>Rule 29</t>
   </si>
   <si>
+    <t>STATION, BEARINGS</t>
+  </si>
+  <si>
+    <t>STATION &gt; 6300</t>
+  </si>
+  <si>
+    <t>STATION &gt; 7330</t>
+  </si>
+  <si>
+    <t>STATION &lt; 9714</t>
+  </si>
+  <si>
+    <t>STATION &lt; 9999</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> starts_with(AAR_CAR_TYPE, "T")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">starts_with(AAR_CAR_TYPE, "V") </t>
+  </si>
+  <si>
+    <t>starts_with(SCS, "112J")</t>
+  </si>
+  <si>
+    <t>AAR_CAR_TYPE,CAR_SERIES,SCS</t>
+  </si>
+  <si>
+    <t>exclude(CAR_SERIES ,"MILW") &lt;= 120209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exclude(CAR_SERIES ,"MILW" )&gt;= 120000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AAR_CAR_TYPE = ['M310','M340']</t>
+  </si>
+  <si>
+    <t>BEARINGS = ['A','C']</t>
+  </si>
+  <si>
+    <t>Rule 57</t>
+  </si>
+  <si>
+    <t>Rule 41,46,42,47</t>
+  </si>
+  <si>
+    <t>******************************************************
+TRAIN HANDLING TANK CARS IN UTLX SERIES.  CARS CANNOT
+MOVE BEYOND NEXT MECHANICAL INSPECTION FACILITY
+******************************************************</t>
+  </si>
+  <si>
     <t>******************************************************
 TRAIN HANDLING TANK CAR(S) WITH PLAIN BEARINGS OR
 ROLLER BEARINGS WITH CONVERTED FRICTION BEARING
 TRUCK SIDEFRAMES.   CARS ARE PROHIBITED IN
-INTERCHANGE OR MOVEMENT ON CPR IF:</t>
-  </si>
-  <si>
-    <t>CONTAINING OR LAST CONTAINED DANGEROUS GOODS
+INTERCHANGE OR MOVEMENT ON CPR IF: CONTAINING OR LAST CONTAINED DANGEROUS GOODS
 ******************************************************</t>
   </si>
   <si>
-    <t>Rule 42,47</t>
-  </si>
-  <si>
-    <t>BEARINGS = ['A','B']</t>
-  </si>
-  <si>
-    <t>STATION, BEARINGS</t>
-  </si>
-  <si>
-    <t>STATION &gt; 6300</t>
-  </si>
-  <si>
-    <t>STATION &gt; 7330</t>
-  </si>
-  <si>
-    <t>STATION &lt; 9714</t>
-  </si>
-  <si>
-    <t>STATION &lt; 9999</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> starts_with(AAR_CAR_TYPE, "T")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">starts_with(AAR_CAR_TYPE, "V") </t>
-  </si>
-  <si>
-    <t>starts_with(SCS, "112J")</t>
-  </si>
-  <si>
-    <t>AAR_CAR_TYPE,CAR_SERIES,SCS</t>
-  </si>
-  <si>
-    <t>exclude(CAR_SERIES ,"MILW") &lt;= 120209</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exclude(CAR_SERIES ,"MILW" )&gt;= 120000 </t>
+    <t>ASSIGNMENT_NUMBER=5000</t>
+  </si>
+  <si>
+    <t>STATION, BEARINGS,ASSIGNMENT_NUMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AAR_CAR_TYPE = 'M530'</t>
+  </si>
+  <si>
+    <t>CAR_SERIES = ['CP  000070','CP  000085', 'CP  000095', 'CP  000096', 'CP  029114', 'CP  401750','CP  401753',  'CP  000099','CP  000102', 'CP  000105', 'CP  000106', 'CP  000110' ]</t>
+  </si>
+  <si>
+    <t>******************************************************
+TRAIN HANDLING BUSINESS CAR(S).
+MUST BE MARSHALLED AS PER GOI SEC 7 ITEM 21.2
+B END TRAILING WHEN PRACTICABLE
+DO NOT EXCEED TIME TABLE FREIGHT TRAIN SPEED  OR AS INDICATED IN GOI SEC 7 ITEM 21.1
+******************************************************</t>
+  </si>
+  <si>
+    <t>Rule 59</t>
+  </si>
+  <si>
+    <t>ASSIGNMENT_NUMBER=2240</t>
+  </si>
+  <si>
+    <t>EMPTY_LOAD = 2</t>
+  </si>
+  <si>
+    <t>Rule 178,179</t>
+  </si>
+  <si>
+    <t>******************************************************
+SOO 4000 4001 4002 AND 4003
+ARE USED TO FUEL LOCOMOTIVES ENROUTE.
+CARS ARE EXEMPT FROM THE
+TRANSPORTATION OF DANGEROUS GOODS REGULATIONS  WHEN MARSHALLED NEXT TO LOCOMOTIVES
+******************************************************</t>
+  </si>
+  <si>
+    <t>STATION = [100, 4544]</t>
+  </si>
+  <si>
+    <t>******************************************************
+TRAIN HANDLING MULTI LEVEL CAR(S) PROHIBITED
+IN BOTH TUBES OF THE DETROIT TUNNEL
+******************************************************</t>
+  </si>
+  <si>
+    <t>Rule 56</t>
+  </si>
+  <si>
+    <t>Rule 250,252</t>
+  </si>
+  <si>
+    <t>starts_with(AAR_CAR_TYPE ,"S*6" )</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> starts_with(AAR_CAR_TYPE ,"S*8" )</t>
+  </si>
+  <si>
+    <t>EMPTY_LOAD = 1</t>
+  </si>
+  <si>
+    <t>******************************************************
+TRAIN HANDLING ARTICULATE MULTI-PLATFORM CAR(S)
+EQUIPPED WITH 125 TON TRUCKS
+LOADED WITH ONE OR MORE CONTAINERS
+IF CONTAINERS ARE DOUBLE STACKED SPEED RESTRICTIONS APPLY PER GOI SECTION 10
+******************************************************</t>
   </si>
 </sst>
 </file>
@@ -523,35 +604,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" customWidth="1"/>
     <col min="4" max="4" width="52.140625" customWidth="1"/>
     <col min="5" max="5" width="43.42578125" customWidth="1"/>
     <col min="6" max="7" width="23.85546875" customWidth="1"/>
     <col min="8" max="8" width="47.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="3" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>6</v>
@@ -598,16 +680,16 @@
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -651,16 +733,16 @@
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>5</v>
@@ -710,10 +792,10 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -760,7 +842,9 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -801,18 +885,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="122.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="182.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="6" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>0</v>
@@ -848,16 +938,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="62.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="122.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>1</v>
@@ -865,7 +955,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="6" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>0</v>
@@ -901,7 +991,223 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:19" ht="137.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="152.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="92.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="152.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed bug for starts_with function
</commit_message>
<xml_diff>
--- a/main/app/brm_core/BRMRulesLatest.xlsx
+++ b/main/app/brm_core/BRMRulesLatest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="47">
   <si>
     <t>None</t>
   </si>
@@ -192,12 +192,6 @@
     <t>Rule 250,252</t>
   </si>
   <si>
-    <t>starts_with(AAR_CAR_TYPE ,"S*6" )</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> starts_with(AAR_CAR_TYPE ,"S*8" )</t>
-  </si>
-  <si>
     <t>EMPTY_LOAD = 1</t>
   </si>
   <si>
@@ -207,6 +201,9 @@
 LOADED WITH ONE OR MORE CONTAINERS
 IF CONTAINERS ARE DOUBLE STACKED SPEED RESTRICTIONS APPLY PER GOI SECTION 10
 ******************************************************</t>
+  </si>
+  <si>
+    <t>starts_with(AAR_CAR_TYPE ,"S*8")  + starts_with(AAR_CAR_TYPE ,"S*6")</t>
   </si>
 </sst>
 </file>
@@ -606,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,24 +1151,22 @@
       <c r="A11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed bug in exclude function
</commit_message>
<xml_diff>
--- a/main/app/brm_core/BRMRulesLatest.xlsx
+++ b/main/app/brm_core/BRMRulesLatest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="47">
-  <si>
-    <t>None</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -50,9 +47,6 @@
     <t xml:space="preserve">EMPTY_LOAD = 2 </t>
   </si>
   <si>
-    <t>EMPTY_LOAD</t>
-  </si>
-  <si>
     <t xml:space="preserve">******************************************************
 TRAIN HANDLING MILW CARS IN SERIES 120000 - 120209
 BRAKE STEP DEFECTIVE.  EXERCISE EXTREME CAUTION
@@ -78,9 +72,6 @@
     <t>Rule 29</t>
   </si>
   <si>
-    <t>STATION, BEARINGS</t>
-  </si>
-  <si>
     <t>STATION &gt; 6300</t>
   </si>
   <si>
@@ -102,13 +93,7 @@
     <t>starts_with(SCS, "112J")</t>
   </si>
   <si>
-    <t>AAR_CAR_TYPE,CAR_SERIES,SCS</t>
-  </si>
-  <si>
     <t>exclude(CAR_SERIES ,"MILW") &lt;= 120209</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exclude(CAR_SERIES ,"MILW" )&gt;= 120000 </t>
   </si>
   <si>
     <t xml:space="preserve"> AAR_CAR_TYPE = ['M310','M340']</t>
@@ -204,6 +189,104 @@
   </si>
   <si>
     <t>starts_with(AAR_CAR_TYPE ,"S*8")  + starts_with(AAR_CAR_TYPE ,"S*6")</t>
+  </si>
+  <si>
+    <t>starts_with(AAR_CAR_TYPE ,"K*8")</t>
+  </si>
+  <si>
+    <t>AAR_CAR_TYPE,CAR_SERIES,SCS,OUTSIDE_LENGTH_FFII</t>
+  </si>
+  <si>
+    <t>OUTSIDE_LENGTH_FFII &gt;2000</t>
+  </si>
+  <si>
+    <t>OUTSIDE_LENGTH_FFII &lt;3001</t>
+  </si>
+  <si>
+    <t>Rule 249</t>
+  </si>
+  <si>
+    <t>Rule 248</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OUTSIDE_LENGTH_FFII &gt;=2500 </t>
+  </si>
+  <si>
+    <t>OUTSIDE_LENGTH_FFII &lt;=3400</t>
+  </si>
+  <si>
+    <t>exclude(CAR_SERIES,"CP")  &gt;= 370000</t>
+  </si>
+  <si>
+    <t>STATION, BEARINGS,CAR_SERIES</t>
+  </si>
+  <si>
+    <t>Rule 15</t>
+  </si>
+  <si>
+    <t>starts_with(AAR_CAR_TYPE ,"M50")</t>
+  </si>
+  <si>
+    <t>******************************************************
+TRAIN MUST NOT OPERATE THROUGH THE MACDONALD TUNNEL
+MOUNTAIN SUBDIVISION UNLESS OTHERWISE AUTHORIZED
+DO NOT COUPLE TO DOUBLE SHELF COUPLER   DO NOT HUMP
+******************************************************</t>
+  </si>
+  <si>
+    <t>******************************************************
+TRAIN HANDLING EQUIPMENT WHICH MUST BE HANDLED
+VIA THE NORTH TUBE OF THE DETROIT TUNNEL
+IF ROUTED THROUGH DETROIT/WINDSOR
+******************************************************</t>
+  </si>
+  <si>
+    <t>STATION&gt;=100</t>
+  </si>
+  <si>
+    <t>STATION&lt;=4544</t>
+  </si>
+  <si>
+    <t>STATION&lt;=498</t>
+  </si>
+  <si>
+    <t>STATION&gt;=454</t>
+  </si>
+  <si>
+    <t>starts_with(AAR_CAR_TYPE ,"V*0") + starts_with(AAR_CAR_TYPE ,"V*1") + starts_with(AAR_CAR_TYPE ,"V*3") + starts_with(AAR_CAR_TYPE ,"V*4") + starts_with(AAR_CAR_TYPE ,"V*6")  +   starts_with(AAR_CAR_TYPE , "V*7")</t>
+  </si>
+  <si>
+    <t>Rule 24,25,26</t>
+  </si>
+  <si>
+    <t>Rule 33,34,36,37</t>
+  </si>
+  <si>
+    <t>CLEARANCE = ['G','F']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">starts_with(AAR_CAR_TYPE ,"A") + starts_with(AAR_CAR_TYPE ,"P") + starts_with(AAR_CAR_TYPE ,"Q") </t>
+  </si>
+  <si>
+    <t>Rule 105</t>
+  </si>
+  <si>
+    <t>AAR_CAR_TYPE,CAR_SERIES,SCS,CLEARANCE</t>
+  </si>
+  <si>
+    <t>OUTSIDE_LENGTH_FFII</t>
+  </si>
+  <si>
+    <t>EMPTY_LOAD,OUTSIDE_LENGTH_FFII</t>
+  </si>
+  <si>
+    <t>CLEARANCE ='F'</t>
+  </si>
+  <si>
+    <t>exclude(CAR_SERIES,"CP")  &lt;= 377349</t>
+  </si>
+  <si>
+    <t>exclude(CAR_SERIES ,"MILW" )&gt;= 120000</t>
   </si>
 </sst>
 </file>
@@ -601,608 +684,379 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
+      <selection activeCell="I12" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="40.85546875" customWidth="1"/>
-    <col min="4" max="4" width="52.140625" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" customWidth="1"/>
-    <col min="6" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="47.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="40.88671875" customWidth="1"/>
+    <col min="4" max="4" width="52.109375" customWidth="1"/>
+    <col min="5" max="5" width="47.44140625" customWidth="1"/>
+    <col min="6" max="7" width="26.5546875" customWidth="1"/>
+    <col min="8" max="8" width="47.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="3" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="80.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="3">
-        <v>0</v>
-      </c>
-      <c r="J1" s="3">
-        <v>0</v>
-      </c>
-      <c r="K1" s="3">
-        <v>0</v>
-      </c>
-      <c r="L1" s="3">
-        <v>0</v>
-      </c>
-      <c r="M1" s="3">
-        <v>0</v>
-      </c>
-      <c r="N1" s="3">
-        <v>0</v>
-      </c>
-      <c r="O1" s="3">
-        <v>0</v>
-      </c>
-      <c r="P1" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="3">
-        <v>0</v>
-      </c>
-      <c r="R1" s="3">
-        <v>0</v>
-      </c>
-      <c r="S1" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="80.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S2" s="1"/>
-    </row>
-    <row r="3" spans="1:19" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="137.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="117" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="102.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="107.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="182.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="174.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="122.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="117" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="137.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="131.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="152.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="145.80000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="92.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="88.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="152.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="145.80000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="145.80000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="H12" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="145.80000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="145.80000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="117" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="117" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="117" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>